<commit_message>
changed excel file to include parsed data
</commit_message>
<xml_diff>
--- a/cs4400_phase2_denormalized_data_v3.xlsx
+++ b/cs4400_phase2_denormalized_data_v3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmoss7/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akhilkammila/Desktop/CS 4400/CS4400 Phase 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BCBA21-0F35-6C47-8DA0-06F9E0697521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215D1753-8B49-B946-9853-85D446457B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52120" yWindow="1100" windowWidth="38700" windowHeight="23700" activeTab="8" xr2:uid="{B8F2E950-D5D2-C646-8BA5-DD2E1BDFCEB7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="8" xr2:uid="{B8F2E950-D5D2-C646-8BA5-DD2E1BDFCEB7}"/>
   </bookViews>
   <sheets>
     <sheet name="airlines" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="577">
   <si>
     <t>index</t>
   </si>
@@ -1822,15 +1822,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2150,19 +2147,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C0CD0F-6286-C74E-874F-128D7D3F5474}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="53.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="53.1640625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="34.83203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2183,8 +2183,12 @@
       <c r="C2" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="1" t="str">
+        <f>"('" &amp; B2 &amp; "','" &amp; C2 &amp; "'),"</f>
+        <v>('Air_France','25'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <f>A2 + 1</f>
         <v>2</v>
@@ -2195,10 +2199,14 @@
       <c r="C3" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="1" t="str">
+        <f t="shared" ref="D3:D9" si="0">"('" &amp; B3 &amp; "','" &amp; C3 &amp; "'),"</f>
+        <v>('American','45'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A9" si="0">A3 + 1</f>
+        <f t="shared" ref="A4:A9" si="1">A3 + 1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2207,10 +2215,14 @@
       <c r="C4" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('Delta','46'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2219,10 +2231,14 @@
       <c r="C5" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('JetBlue','8'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2231,10 +2247,14 @@
       <c r="C6" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('Lufthansa','31'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2243,10 +2263,14 @@
       <c r="C7" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('Southwest','22'),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2255,10 +2279,14 @@
       <c r="C8" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('Spirit','4'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2266,6 +2294,10 @@
       </c>
       <c r="C9" s="1">
         <v>40</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('United','40'),</v>
       </c>
     </row>
   </sheetData>
@@ -2275,9 +2307,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC785781-21C3-8C41-B8DA-E4E84F4CC964}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39"/>
   <cols>
@@ -2286,7 +2320,7 @@
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2294,180 +2328,272 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="1" t="str">
+        <f>"("
+&amp; IF(ISBLANK(B2),"NULL",_xlfn.CONCAT("'",B2,"'"))
+&amp; "),"</f>
+        <v>('plane_1'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="1" t="str">
+        <f t="shared" ref="C3:C23" si="0">"("
+&amp; IF(ISBLANK(B3),"NULL",_xlfn.CONCAT("'",B3,"'"))
+&amp; "),"</f>
+        <v>('plane_11'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('plane_15'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('plane_2'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('plane_4'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('plane_7'),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('plane_8'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('plane_9'),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('port_1'),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('port_10'),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('port_11'),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('port_13'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('port_14'),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('port_15'),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('port_17'),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('port_18'),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('port_2'),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('port_3'),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('port_4'),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('port_5'),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('port_7'),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>527</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('port_9'),</v>
       </c>
     </row>
   </sheetData>
@@ -2477,9 +2603,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD1BC1A6-A1CA-014D-BFE5-F14821E05CB8}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E5" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39"/>
   <cols>
@@ -2492,10 +2620,11 @@
     <col min="7" max="7" width="21.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.1640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="23.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="78.33203125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2524,7 +2653,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2549,8 +2678,21 @@
       <c r="I2" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="1" t="str">
+        <f>"("
+&amp; IF(ISBLANK(B2),"NULL",_xlfn.CONCAT("'",B2,"'")) &amp; ","
+&amp; IF(ISBLANK(C2),"NULL",_xlfn.CONCAT("'",C2,"'")) &amp; ","
+&amp; IF(ISBLANK(D2),"NULL",_xlfn.CONCAT("'",D2,"'")) &amp; ","
+&amp; IF(ISBLANK(E2),"NULL",_xlfn.CONCAT("'",E2,"'")) &amp; ","
+&amp; IF(ISBLANK(F2),"NULL",_xlfn.CONCAT("'",F2,"'")) &amp; ","
+&amp; IF(ISBLANK(G2),"NULL",_xlfn.CONCAT("'",G2,"'")) &amp; ","
+&amp; IF(ISBLANK(H2),"NULL",_xlfn.CONCAT("'",H2,"'")) &amp; ","
+&amp; IF(ISBLANK(I2),"NULL",_xlfn.CONCAT("'",I2,"'"))
+&amp; "),"</f>
+        <v>('American','n330ss','4','200','plane_4','jet',NULL,'2'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2572,8 +2714,21 @@
       <c r="I3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="1" t="str">
+        <f t="shared" ref="J3:J18" si="0">"("
+&amp; IF(ISBLANK(B3),"NULL",_xlfn.CONCAT("'",B3,"'")) &amp; ","
+&amp; IF(ISBLANK(C3),"NULL",_xlfn.CONCAT("'",C3,"'")) &amp; ","
+&amp; IF(ISBLANK(D3),"NULL",_xlfn.CONCAT("'",D3,"'")) &amp; ","
+&amp; IF(ISBLANK(E3),"NULL",_xlfn.CONCAT("'",E3,"'")) &amp; ","
+&amp; IF(ISBLANK(F3),"NULL",_xlfn.CONCAT("'",F3,"'")) &amp; ","
+&amp; IF(ISBLANK(G3),"NULL",_xlfn.CONCAT("'",G3,"'")) &amp; ","
+&amp; IF(ISBLANK(H3),"NULL",_xlfn.CONCAT("'",H3,"'")) &amp; ","
+&amp; IF(ISBLANK(I3),"NULL",_xlfn.CONCAT("'",I3,"'"))
+&amp; "),"</f>
+        <v>('American','n380sd','5','400',NULL,'jet',NULL,'2'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2598,8 +2753,12 @@
       <c r="I4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('Delta','n106js','4','200','plane_1','jet',NULL,'2'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2624,8 +2783,12 @@
       <c r="I5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('Delta','n110jn','5','600','plane_2','jet',NULL,'4'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2641,8 +2804,12 @@
       <c r="E6" s="1">
         <v>800</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('Delta','n127js','4','800',NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2658,8 +2825,12 @@
       <c r="E7" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('Delta','n156sq','8','100',NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2681,8 +2852,12 @@
       <c r="I8" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('JetBlue','n161fk','4','200',NULL,'jet',NULL,'2'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2704,8 +2879,12 @@
       <c r="I9" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('JetBlue','n337as','5','400',NULL,'jet',NULL,'2'),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2733,8 +2912,12 @@
       <c r="I10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('Southwest','n118fm','4','100','plane_11','prop','1','1'),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2759,8 +2942,12 @@
       <c r="I11" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('Southwest','n401fj','4','200','plane_9','jet',NULL,'2'),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2782,8 +2969,12 @@
       <c r="I12" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('Southwest','n653fk','6','400',NULL,'jet',NULL,'2'),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2808,8 +2999,12 @@
       <c r="I13" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('Southwest','n815pw','3','200',NULL,'prop','0','2'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2834,8 +3029,12 @@
       <c r="I14" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('Spirit','n256ap','4','400','plane_15','jet',NULL,'2'),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2857,8 +3056,12 @@
       <c r="I15" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('United','n451fi','5','400',NULL,'jet',NULL,'4'),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2883,8 +3086,12 @@
       <c r="I16" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('United','n517ly','4','400','plane_7','jet',NULL,'2'),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2906,8 +3113,12 @@
       <c r="I17" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('United','n616lt','7','400',NULL,'jet',NULL,'4'),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2934,6 +3145,10 @@
       </c>
       <c r="I18" s="1">
         <v>2</v>
+      </c>
+      <c r="J18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('United','n620la','4','200','plane_8','prop','0','2'),</v>
       </c>
     </row>
   </sheetData>
@@ -2943,9 +3158,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7063475-3288-0147-86E0-B70C596A4991}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0"/>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39"/>
   <cols>
@@ -2955,10 +3172,11 @@
     <col min="4" max="4" width="44.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="33.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="23.1640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="106.33203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2978,7 +3196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2994,8 +3212,18 @@
       <c r="E2" s="1" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="1" t="str">
+        <f>"("
+&amp; IF(ISBLANK(B2),"NULL",_xlfn.CONCAT("'",B2,"'")) &amp; ","
+&amp; IF(ISBLANK(C2),"NULL",_xlfn.CONCAT("'",C2,"'")) &amp; ","
+&amp; IF(ISBLANK(D2),"NULL",_xlfn.CONCAT("'",D2,"'")) &amp; ","
+&amp; IF(ISBLANK(E2),"NULL",_xlfn.CONCAT("'",E2,"'")) &amp; ","
+&amp; IF(ISBLANK(F2),"NULL",_xlfn.CONCAT("'",F2,"'"))
+&amp; "),"</f>
+        <v>('ABQ','Albuquerque International Sunport','Albuquerque','NM',NULL),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3011,8 +3239,18 @@
       <c r="E3" s="1" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="1" t="str">
+        <f t="shared" ref="G3:G64" si="0">"("
+&amp; IF(ISBLANK(B3),"NULL",_xlfn.CONCAT("'",B3,"'")) &amp; ","
+&amp; IF(ISBLANK(C3),"NULL",_xlfn.CONCAT("'",C3,"'")) &amp; ","
+&amp; IF(ISBLANK(D3),"NULL",_xlfn.CONCAT("'",D3,"'")) &amp; ","
+&amp; IF(ISBLANK(E3),"NULL",_xlfn.CONCAT("'",E3,"'")) &amp; ","
+&amp; IF(ISBLANK(F3),"NULL",_xlfn.CONCAT("'",F3,"'"))
+&amp; "),"</f>
+        <v>('ANC','Ted Stevens Anchorage International Airport','Anchorage','AK',NULL),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3031,8 +3269,12 @@
       <c r="F4" s="1" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('ATL','Hartsfield-Jackson Atlanta International Airport','Atlanta','GA','port_1'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3048,8 +3290,12 @@
       <c r="E5" s="1" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('BDL','Bradley International Airport','Hartford','CT',NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3068,8 +3314,12 @@
       <c r="F6" s="1" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('BFI','King County International Airport','Seattle','WA','port_10'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3085,8 +3335,12 @@
       <c r="E7" s="1" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('BHM','Birmingham-Shuttlesworth International Airport','Birmingham','AL',NULL),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3102,8 +3356,12 @@
       <c r="E8" s="1" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('BNA','Nashville International Airport','Nashville','TN',NULL),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3119,8 +3377,12 @@
       <c r="E9" s="1" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('BOI','Boise Airport ','Boise','ID',NULL),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3136,8 +3398,12 @@
       <c r="E10" s="1" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('BOS','General Edward Lawrence Logan International Airport','Boston','MA',NULL),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3153,8 +3419,12 @@
       <c r="E11" s="1" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('BTV','Burlington International Airport','Burlington','VT',NULL),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3170,8 +3440,12 @@
       <c r="E12" s="1" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('BWI','Baltimore_Washington International Airport','Baltimore','MD',NULL),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3187,8 +3461,12 @@
       <c r="E13" s="1" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('BZN','Bozeman Yellowstone International Airport','Bozeman','MT',NULL),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3204,8 +3482,12 @@
       <c r="E14" s="1" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('CHS','Charleston International Airport','Charleston','SC',NULL),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3221,8 +3503,12 @@
       <c r="E15" s="1" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('CLE','Cleveland Hopkins International Airport','Cleveland','OH',NULL),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3238,8 +3524,12 @@
       <c r="E16" s="1" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('CLT','Charlotte Douglas International Airport','Charlotte','NC',NULL),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3255,8 +3545,12 @@
       <c r="E17" s="1" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('CRW','Yeager Airport','Charleston','WV',NULL),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3275,8 +3569,12 @@
       <c r="F18" s="1" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('DAL','Dallas Love Field','Dallas','TX','port_7'),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3295,8 +3593,12 @@
       <c r="F19" s="1" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('DCA','Ronald Reagan Washington National Airport','Washington','DC','port_9'),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3315,8 +3617,12 @@
       <c r="F20" s="1" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('DEN','Denver International Airport','Denver','CO','port_3'),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3335,8 +3641,12 @@
       <c r="F21" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('DFW','Dallas-Fort Worth International Airport','Dallas','TX','port_2'),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3352,8 +3662,12 @@
       <c r="E22" s="1" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('DSM','Des Moines International Airport','Des Moines','IA',NULL),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3369,8 +3683,12 @@
       <c r="E23" s="1" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('DTW','Detroit Metro Wayne County Airport','Detroit','MI',NULL),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3386,8 +3704,12 @@
       <c r="E24" s="1" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('EWR','Newark Liberty International Airport','Newark','NJ',NULL),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3403,8 +3725,12 @@
       <c r="E25" s="1" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('FAR','Hector International Airport','Fargo','ND',NULL),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3420,8 +3746,12 @@
       <c r="E26" s="1" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('FSD','Joe Foss Field','Sioux Falls','SD',NULL),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3437,8 +3767,12 @@
       <c r="E27" s="1" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('GSN','Saipan International Airport','Obyan Saipan Island','MP',NULL),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3454,8 +3788,12 @@
       <c r="E28" s="1" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('GUM','Antonio B_Won Pat International Airport','Agana Tamuning','GU',NULL),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3471,8 +3809,12 @@
       <c r="E29" s="1" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('HNL','Daniel K. Inouye International Airport','Honolulu Oahu','HI',NULL),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3491,8 +3833,12 @@
       <c r="F30" s="1" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('HOU','William P_Hobby Airport','Houston','TX','port_18'),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3511,8 +3857,12 @@
       <c r="F31" s="1" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('IAD','Washington Dulles International Airport','Washington','DC','port_11'),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -3531,8 +3881,12 @@
       <c r="F32" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('IAH','George Bush Intercontinental Houston Airport','Houston','TX','port_13'),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -3548,8 +3902,12 @@
       <c r="E33" s="1" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('ICT','Wichita Dwight D_Eisenhower National Airport ','Wichita','KS',NULL),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -3565,8 +3923,12 @@
       <c r="E34" s="1" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('ILG','Wilmington Airport','Wilmington','DE',NULL),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3582,8 +3944,12 @@
       <c r="E35" s="1" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('IND','Indianapolis International Airport','Indianapolis','IN',NULL),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -3602,8 +3968,12 @@
       <c r="F36" s="1" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('ISP','Long Island MacArthur Airport','New York Islip','NY','port_14'),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -3619,8 +3989,12 @@
       <c r="E37" s="1" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('JAC','Jackson Hole Airport','Jackson','WY',NULL),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3636,8 +4010,12 @@
       <c r="E38" s="1" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('JAN','Jackson_Medgar Wiley Evers International Airport','Jackson','MS',NULL),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3656,8 +4034,12 @@
       <c r="F39" s="1" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('JFK','John F_Kennedy International Airport ','New York','NY','port_15'),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3673,8 +4055,12 @@
       <c r="E40" s="1" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('LAS','Harry Reid International Airport','Las Vegas','NV',NULL),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3693,8 +4079,12 @@
       <c r="F41" s="1" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('LAX','Los Angeles International Airport','Los Angeles','CA','port_5'),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3710,8 +4100,12 @@
       <c r="E42" s="1" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('LGA','LaGuardia Airport','New York','NY',NULL),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3727,8 +4121,12 @@
       <c r="E43" s="1" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('LIT','Bill and Hillary Clinton National Airport','Little Rock','AR',NULL),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3744,8 +4142,12 @@
       <c r="E44" s="1" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('MCO','Orlando International Airport','Orlando','FL',NULL),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3761,8 +4163,12 @@
       <c r="E45" s="1" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('MDW','Chicago Midway International Airport','Chicago','IL',NULL),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3778,8 +4184,12 @@
       <c r="E46" s="1" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('MHT','Manchester_Boston Regional Airport','Manchester','NH',NULL),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3795,8 +4205,12 @@
       <c r="E47" s="1" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('MKE','Milwaukee Mitchell International Airport','Milwaukee','WI',NULL),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3812,8 +4226,12 @@
       <c r="E48" s="1" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('MRI','Merrill Field','Anchorage','AK',NULL),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3829,8 +4247,12 @@
       <c r="E49" s="1" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('MSP','Minneapolis_St_Paul International Wold_Chamberlain Airport','Minneapolis Saint Paul','MN',NULL),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3846,8 +4268,12 @@
       <c r="E50" s="1" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('MSY','Louis Armstrong New Orleans International Airport','New Orleans','LA',NULL),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3863,8 +4289,12 @@
       <c r="E51" s="1" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('OKC','Will Rogers World Airport','Oklahoma City','OK',NULL),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3880,8 +4310,12 @@
       <c r="E52" s="1" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('OMA','Eppley Airfield','Omaha','NE',NULL),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3900,8 +4334,12 @@
       <c r="F53" s="1" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('ORD','O_Hare International Airport','Chicago','IL','port_4'),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3917,8 +4355,12 @@
       <c r="E54" s="1" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('PDX','Portland International Airport','Portland','OR',NULL),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3934,8 +4376,12 @@
       <c r="E55" s="1" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('PHL','Philadelphia International Airport','Philadelphia','PA',NULL),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3951,8 +4397,12 @@
       <c r="E56" s="1" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('PHX','Phoenix Sky Harbor International Airport','Phoenix','AZ',NULL),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3968,8 +4418,12 @@
       <c r="E57" s="1" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('PVD','Rhode Island T_F_Green International Airport','Providence','RI',NULL),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3985,8 +4439,12 @@
       <c r="E58" s="1" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('PWM','Portland International Jetport','Portland','ME',NULL),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -4002,8 +4460,12 @@
       <c r="E59" s="1" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('SDF','Louisville International Airport','Louisville','KY',NULL),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -4022,8 +4484,12 @@
       <c r="F60" s="1" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('SEA','Seattle-Tacoma International Airport','Seattle Tacoma','WA','port_17'),</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -4039,8 +4505,12 @@
       <c r="E61" s="1" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('SJU','Luis Munoz Marin International Airport','San Juan Carolina','PR',NULL),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -4056,8 +4526,12 @@
       <c r="E62" s="1" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('SLC','Salt Lake City International Airport','Salt Lake City','UT',NULL),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -4073,8 +4547,12 @@
       <c r="E63" s="1" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('STL','St_Louis Lambert International Airport','Saint Louis','MO',NULL),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -4089,6 +4567,10 @@
       </c>
       <c r="E64" s="1" t="s">
         <v>514</v>
+      </c>
+      <c r="G64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('STT','Cyril E_King Airport','Charlotte Amalie Saint Thomas','VI',NULL),</v>
       </c>
     </row>
   </sheetData>
@@ -4098,9 +4580,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE4A992-160B-C34E-BC16-5248D945800B}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="I36" workbookViewId="0">
+      <selection activeCell="O48" sqref="O48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39"/>
   <cols>
@@ -4117,7 +4601,7 @@
     <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="39" customHeight="1">
+    <row r="1" spans="1:14" ht="39" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4158,7 +4642,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="39" customHeight="1">
+    <row r="2" spans="1:14" ht="39" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4192,11 +4676,25 @@
       <c r="L2" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="39" customHeight="1">
+      <c r="N2" s="1" t="str">
+        <f>"("
+&amp; IF(ISBLANK(B2),"NULL",_xlfn.CONCAT("'",B2,"'")) &amp; ","
+&amp; IF(ISBLANK(C2),"NULL",_xlfn.CONCAT("'",C2,"'")) &amp; ","
+&amp; IF(ISBLANK(D2),"NULL",_xlfn.CONCAT("'",D2,"'")) &amp; ","
+&amp; IF(ISBLANK(E2),"NULL",_xlfn.CONCAT("'",E2,"'")) &amp; ","
+&amp; IF(ISBLANK(F2),"NULL",_xlfn.CONCAT("'",F2,"'")) &amp; ","
+&amp; IF(ISBLANK(G2),"NULL",_xlfn.CONCAT("'",G2,"'")) &amp; ","
+&amp; IF(ISBLANK(H2),"NULL",_xlfn.CONCAT("'",H2,"'")) &amp; ","
+&amp; IF(ISBLANK(I2),"NULL",_xlfn.CONCAT("'",I2,"'")) &amp; ","
+&amp; IF(ISBLANK(J2),"NULL",_xlfn.CONCAT("'",J2,"'")) &amp; ","
+&amp; IF(ISBLANK(K2),"NULL",_xlfn.CONCAT("'",K2,"'")) &amp; ","
+&amp; IF(ISBLANK(L2),"NULL",_xlfn.CONCAT("'",L2,"'")) &amp; ","
+&amp; IF(ISBLANK(M2),"NULL",_xlfn.CONCAT("'",M2,"'"))
+&amp; "),"</f>
+        <v>('p1','Jeanne','Nelson','plane_1','330-12-6907','31','Delta','n106js',NULL,'jet','',NULL),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="39" customHeight="1">
       <c r="A3" s="1">
         <f>A2 + 1</f>
         <v>2</v>
@@ -4234,10 +4732,27 @@
       <c r="M3" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="39" customHeight="1">
+      <c r="N3" s="1" t="str">
+        <f t="shared" ref="N3:N46" si="0">"("
+&amp; IF(ISBLANK(B3),"NULL",_xlfn.CONCAT("'",B3,"'")) &amp; ","
+&amp; IF(ISBLANK(C3),"NULL",_xlfn.CONCAT("'",C3,"'")) &amp; ","
+&amp; IF(ISBLANK(D3),"NULL",_xlfn.CONCAT("'",D3,"'")) &amp; ","
+&amp; IF(ISBLANK(E3),"NULL",_xlfn.CONCAT("'",E3,"'")) &amp; ","
+&amp; IF(ISBLANK(F3),"NULL",_xlfn.CONCAT("'",F3,"'")) &amp; ","
+&amp; IF(ISBLANK(G3),"NULL",_xlfn.CONCAT("'",G3,"'")) &amp; ","
+&amp; IF(ISBLANK(H3),"NULL",_xlfn.CONCAT("'",H3,"'")) &amp; ","
+&amp; IF(ISBLANK(I3),"NULL",_xlfn.CONCAT("'",I3,"'")) &amp; ","
+&amp; IF(ISBLANK(J3),"NULL",_xlfn.CONCAT("'",J3,"'")) &amp; ","
+&amp; IF(ISBLANK(K3),"NULL",_xlfn.CONCAT("'",K3,"'")) &amp; ","
+&amp; IF(ISBLANK(L3),"NULL",_xlfn.CONCAT("'",L3,"'")) &amp; ","
+&amp; IF(ISBLANK(M3),"NULL",_xlfn.CONCAT("'",M3,"'"))
+&amp; "),"</f>
+        <v>('p10','Lawrence','Morgan','plane_9','769-60-1266','15','Southwest','n401fj',NULL,'jet','',''),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="39" customHeight="1">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A46" si="0">A3 + 1</f>
+        <f t="shared" ref="A4:A46" si="1">A3 + 1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -4273,10 +4788,14 @@
       <c r="M4" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="39" customHeight="1">
+      <c r="N4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p11','Sandra','Cruz','plane_9','369-22-9505','22','Southwest','n401fj',NULL,'jet','prop',''),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="39" customHeight="1">
       <c r="A5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -4312,10 +4831,14 @@
       <c r="M5" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="39" customHeight="1">
+      <c r="N5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p12','Dan','Ball','plane_11','680-92-5329','24','Southwest','n118fm',NULL,'prop','',''),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="39" customHeight="1">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -4351,10 +4874,14 @@
       <c r="M6" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="39" customHeight="1">
+      <c r="N6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p13','Bryant','Figueroa','plane_2','513-40-4168','24','Delta','n110jn',NULL,'jet','',''),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="39" customHeight="1">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -4390,10 +4917,14 @@
       <c r="M7" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="39" customHeight="1">
+      <c r="N7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p14','Dana','Perry','plane_2','454-71-7847','13','Delta','n110jn',NULL,'jet','',''),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="39" customHeight="1">
       <c r="A8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -4429,10 +4960,14 @@
       <c r="M8" s="1" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="39" customHeight="1">
+      <c r="N8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p15','Matt','Hunt','plane_2','153-47-8101','30','Delta','n110jn',NULL,'jet','prop','testing'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="39" customHeight="1">
       <c r="A9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -4468,10 +5003,14 @@
       <c r="M9" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="39" customHeight="1">
+      <c r="N9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p16','Edna','Brown','plane_15','598-47-5172','28','Spirit','n256ap',NULL,'jet','',''),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="39" customHeight="1">
       <c r="A10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -4507,10 +5046,14 @@
       <c r="M10" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="39" customHeight="1">
+      <c r="N10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p17','Ruby','Burgess','plane_15','865-71-6800','36','Spirit','n256ap',NULL,'jet','prop',''),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="39" customHeight="1">
       <c r="A11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -4540,10 +5083,14 @@
       <c r="M11" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="39" customHeight="1">
+      <c r="N11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p18','Esther','Pittman','port_2','250-86-2784','23',NULL,NULL,NULL,'jet','',''),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="39" customHeight="1">
       <c r="A12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -4573,10 +5120,14 @@
       <c r="M12" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="39" customHeight="1">
+      <c r="N12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p19','Doug','Fowler','port_4','386-39-7881','2',NULL,NULL,NULL,'jet','',''),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="39" customHeight="1">
       <c r="A13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -4612,10 +5163,14 @@
       <c r="M13" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="39" customHeight="1">
+      <c r="N13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p2','Roxanne','Byrd','plane_1','842-88-1257','9','Delta','n106js',NULL,'jet','prop',''),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="39" customHeight="1">
       <c r="A14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -4645,10 +5200,14 @@
       <c r="M14" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="39" customHeight="1">
+      <c r="N14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p20','Thomas','Olson','port_3','522-44-3098','28',NULL,NULL,NULL,'jet','',''),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="39" customHeight="1">
       <c r="A15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -4681,10 +5240,14 @@
       <c r="M15" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="39" customHeight="1">
+      <c r="N15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p21','Mona','Harrison','port_4','621-34-5755','2',NULL,NULL,'771','jet','prop',''),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="39" customHeight="1">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -4717,10 +5280,14 @@
       <c r="M16" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="39" customHeight="1">
+      <c r="N16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p22','Arlene','Massey','port_2','177-47-9877','3',NULL,NULL,'374','jet','',''),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="39" customHeight="1">
       <c r="A17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -4753,10 +5320,14 @@
       <c r="M17" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="39" customHeight="1">
+      <c r="N17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p23','Judith','Patrick','port_3','528-64-7912','12',NULL,NULL,'414','jet','',''),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="39" customHeight="1">
       <c r="A18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -4789,10 +5360,14 @@
       <c r="M18" s="1" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="39" customHeight="1">
+      <c r="N18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p24','Reginald','Rhodes','plane_1','803-30-1789','34',NULL,NULL,'292','jet','prop','testing'),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="39" customHeight="1">
       <c r="A19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -4825,10 +5400,14 @@
       <c r="M19" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="39" customHeight="1">
+      <c r="N19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p25','Vincent','Garcia','plane_1','986-76-1587','13',NULL,NULL,'390','jet','',''),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="39" customHeight="1">
       <c r="A20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -4861,10 +5440,14 @@
       <c r="M20" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="39" customHeight="1">
+      <c r="N20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p26','Cheryl','Moore','plane_4','584-77-5105','20',NULL,NULL,'302','jet','',''),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="39" customHeight="1">
       <c r="A21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -4891,10 +5474,14 @@
       <c r="M21" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="39" customHeight="1">
+      <c r="N21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p27','Michael','Rivera','plane_7',NULL,NULL,NULL,NULL,'470','','',''),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="39" customHeight="1">
       <c r="A22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -4921,10 +5508,14 @@
       <c r="M22" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="39" customHeight="1">
+      <c r="N22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p28','Luther','Matthews','plane_8',NULL,NULL,NULL,NULL,'208','','',''),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="39" customHeight="1">
       <c r="A23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -4951,10 +5542,14 @@
       <c r="M23" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="39" customHeight="1">
+      <c r="N23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p29','Moses','Parks','plane_8',NULL,NULL,NULL,NULL,'292','','',''),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="39" customHeight="1">
       <c r="A24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -4990,10 +5585,14 @@
       <c r="M24" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="39" customHeight="1">
+      <c r="N24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p3','Tanya','Nguyen','plane_4','750-24-7616','11','American','n330ss',NULL,'jet','',''),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="39" customHeight="1">
       <c r="A25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -5020,10 +5619,14 @@
       <c r="M25" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="39" customHeight="1">
+      <c r="N25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p30','Ora','Steele','plane_9',NULL,NULL,NULL,NULL,'686','','',''),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="39" customHeight="1">
       <c r="A26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -5050,10 +5653,14 @@
       <c r="M26" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="39" customHeight="1">
+      <c r="N26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p31','Antonio','Flores','plane_9',NULL,NULL,NULL,NULL,'547','','',''),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="39" customHeight="1">
       <c r="A27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -5080,10 +5687,14 @@
       <c r="M27" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="39" customHeight="1">
+      <c r="N27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p32','Glenn','Ross','plane_11',NULL,NULL,NULL,NULL,'257','','',''),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="39" customHeight="1">
       <c r="A28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -5110,10 +5721,14 @@
       <c r="M28" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="39" customHeight="1">
+      <c r="N28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p33','Irma','Thomas','plane_11',NULL,NULL,NULL,NULL,'564','','',''),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="39" customHeight="1">
       <c r="A29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -5140,10 +5755,14 @@
       <c r="M29" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="39" customHeight="1">
+      <c r="N29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p34','Ann','Maldonado','plane_2',NULL,NULL,NULL,NULL,'211','','',''),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="39" customHeight="1">
       <c r="A30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -5170,10 +5789,14 @@
       <c r="M30" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="39" customHeight="1">
+      <c r="N30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p35','Jeffrey','Cruz','plane_2',NULL,NULL,NULL,NULL,'233','','',''),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="39" customHeight="1">
       <c r="A31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -5200,10 +5823,14 @@
       <c r="M31" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="39" customHeight="1">
+      <c r="N31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p36','Sonya','Price','plane_15',NULL,NULL,NULL,NULL,'293','','',''),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="39" customHeight="1">
       <c r="A32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -5230,10 +5857,14 @@
       <c r="M32" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" ht="39" customHeight="1">
+      <c r="N32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p37','Tracy','Hale','plane_15',NULL,NULL,NULL,NULL,'552','','',''),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="39" customHeight="1">
       <c r="A33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -5260,10 +5891,14 @@
       <c r="M33" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" ht="39" customHeight="1">
+      <c r="N33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p38','Albert','Simmons','port_1',NULL,NULL,NULL,NULL,'812','','',''),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="39" customHeight="1">
       <c r="A34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -5290,10 +5925,14 @@
       <c r="M34" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" ht="39" customHeight="1">
+      <c r="N34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p39','Karen','Terry','port_9',NULL,NULL,NULL,NULL,'541','','',''),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="39" customHeight="1">
       <c r="A35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -5329,10 +5968,14 @@
       <c r="M35" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" ht="39" customHeight="1">
+      <c r="N35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p4','Kendra','Jacobs','plane_4','776-21-8098','24','American','n330ss',NULL,'jet','prop',''),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="39" customHeight="1">
       <c r="A36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -5359,10 +6002,14 @@
       <c r="M36" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" ht="39" customHeight="1">
+      <c r="N36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p40','Glen','Kelley','plane_4',NULL,NULL,NULL,NULL,'441','','',''),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="39" customHeight="1">
       <c r="A37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -5389,10 +6036,14 @@
       <c r="M37" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" ht="39" customHeight="1">
+      <c r="N37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p41','Brooke','Little','port_4',NULL,NULL,NULL,NULL,'875','','',''),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="39" customHeight="1">
       <c r="A38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -5419,10 +6070,14 @@
       <c r="M38" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" ht="39" customHeight="1">
+      <c r="N38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p42','Daryl','Nguyen','port_3',NULL,NULL,NULL,NULL,'691','','',''),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="39" customHeight="1">
       <c r="A39" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -5449,10 +6104,14 @@
       <c r="M39" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" ht="39" customHeight="1">
+      <c r="N39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p43','Judy','Willis','port_1',NULL,NULL,NULL,NULL,'572','','',''),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="39" customHeight="1">
       <c r="A40" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -5479,10 +6138,14 @@
       <c r="M40" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" ht="39" customHeight="1">
+      <c r="N40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p44','Marco','Klein','port_2',NULL,NULL,NULL,NULL,'572','','',''),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="39" customHeight="1">
       <c r="A41" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -5509,10 +6172,14 @@
       <c r="M41" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" ht="39" customHeight="1">
+      <c r="N41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p45','Angelica','Hampton','port_5',NULL,NULL,NULL,NULL,'663','','',''),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="39" customHeight="1">
       <c r="A42" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -5548,10 +6215,14 @@
       <c r="M42" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" ht="39" customHeight="1">
+      <c r="N42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p5','Jeff','Burton','plane_4','933-93-2165','27','American','n330ss',NULL,'jet','',''),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="39" customHeight="1">
       <c r="A43" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -5587,10 +6258,14 @@
       <c r="M43" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" ht="39" customHeight="1">
+      <c r="N43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p6','Randal','Parks','plane_7','707-84-4555','38','United','n517ly',NULL,'jet','prop',''),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="39" customHeight="1">
       <c r="A44" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -5626,10 +6301,14 @@
       <c r="M44" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" ht="39" customHeight="1">
+      <c r="N44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p7','Sonya','Owens','plane_7','450-25-5617','13','United','n517ly',NULL,'jet','',''),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="39" customHeight="1">
       <c r="A45" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -5665,10 +6344,14 @@
       <c r="M45" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" ht="39" customHeight="1">
+      <c r="N45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p8','Bennie','Palmer','plane_8','701-38-2179','12','United','n620la',NULL,'prop','',''),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="39" customHeight="1">
       <c r="A46" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -5703,6 +6386,10 @@
       </c>
       <c r="M46" s="1" t="s">
         <v>440</v>
+      </c>
+      <c r="N46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('p9','Marlene','Warner','plane_8','936-44-6941','13','United','n620la',NULL,'jet','prop','testing'),</v>
       </c>
     </row>
   </sheetData>
@@ -5712,9 +6399,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8619C3A9-6514-A946-8697-951A69ADFCED}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39"/>
   <cols>
@@ -5724,7 +6413,7 @@
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39" customHeight="1">
+    <row r="1" spans="1:13" ht="39" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5762,7 +6451,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="39" customHeight="1">
+    <row r="2" spans="1:13" ht="39" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -5799,8 +6488,24 @@
       <c r="L2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="39" customHeight="1">
+      <c r="M2" s="1" t="str">
+        <f>"("
+&amp; IF(ISBLANK(B2),"NULL",_xlfn.CONCAT("'",B2,"'")) &amp; ","
+&amp; IF(ISBLANK(C2),"NULL",_xlfn.CONCAT("'",C2,"'")) &amp; ","
+&amp; IF(ISBLANK(D2),"NULL",_xlfn.CONCAT("'",D2,"'")) &amp; ","
+&amp; IF(ISBLANK(E2),"NULL",_xlfn.CONCAT("'",E2,"'")) &amp; ","
+&amp; IF(ISBLANK(F2),"NULL",_xlfn.CONCAT("'",F2,"'")) &amp; ","
+&amp; IF(ISBLANK(G2),"NULL",_xlfn.CONCAT("'",G2,"'")) &amp; ","
+&amp; IF(ISBLANK(H2),"NULL",_xlfn.CONCAT("'",H2,"'")) &amp; ","
+&amp; IF(ISBLANK(I2),"NULL",_xlfn.CONCAT("'",I2,"'")) &amp; ","
+&amp; IF(ISBLANK(J2),"NULL",_xlfn.CONCAT("'",J2,"'")) &amp; ","
+&amp; IF(ISBLANK(K2),"NULL",_xlfn.CONCAT("'",K2,"'")) &amp; ","
+&amp; IF(ISBLANK(L2),"NULL",_xlfn.CONCAT("'",L2,"'"))
+&amp; "),"</f>
+        <v>('circle_east_coast','ATL','leg_4','600','ORD','leg_20','600','DCA','leg_7','600','ATL'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="39" customHeight="1">
       <c r="A3" s="1">
         <f>A2 + 1</f>
         <v>2</v>
@@ -5838,10 +6543,26 @@
       <c r="L3" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="39" customHeight="1">
+      <c r="M3" s="1" t="str">
+        <f t="shared" ref="M3:M13" si="0">"("
+&amp; IF(ISBLANK(B3),"NULL",_xlfn.CONCAT("'",B3,"'")) &amp; ","
+&amp; IF(ISBLANK(C3),"NULL",_xlfn.CONCAT("'",C3,"'")) &amp; ","
+&amp; IF(ISBLANK(D3),"NULL",_xlfn.CONCAT("'",D3,"'")) &amp; ","
+&amp; IF(ISBLANK(E3),"NULL",_xlfn.CONCAT("'",E3,"'")) &amp; ","
+&amp; IF(ISBLANK(F3),"NULL",_xlfn.CONCAT("'",F3,"'")) &amp; ","
+&amp; IF(ISBLANK(G3),"NULL",_xlfn.CONCAT("'",G3,"'")) &amp; ","
+&amp; IF(ISBLANK(H3),"NULL",_xlfn.CONCAT("'",H3,"'")) &amp; ","
+&amp; IF(ISBLANK(I3),"NULL",_xlfn.CONCAT("'",I3,"'")) &amp; ","
+&amp; IF(ISBLANK(J3),"NULL",_xlfn.CONCAT("'",J3,"'")) &amp; ","
+&amp; IF(ISBLANK(K3),"NULL",_xlfn.CONCAT("'",K3,"'")) &amp; ","
+&amp; IF(ISBLANK(L3),"NULL",_xlfn.CONCAT("'",L3,"'"))
+&amp; "),"</f>
+        <v>('circle_west_coast','LAX','leg_18','1200','DFW','leg_10','800','ORD','leg_22','800','LAX'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="39" customHeight="1">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A14" si="0">A3 + 1</f>
+        <f t="shared" ref="A4:A14" si="1">A3 + 1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -5877,10 +6598,14 @@
       <c r="L4" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="39" customHeight="1">
+      <c r="M4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('eastbound_north_milk_run','SEA','leg_24','1800','ORD','leg_20','600','DCA','leg_8','200','JFK'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="39" customHeight="1">
       <c r="A5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -5898,10 +6623,14 @@
       <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="39" customHeight="1">
+      <c r="M5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('eastbound_north_nonstop','SEA','leg_23','2400','JFK',NULL,NULL,NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="39" customHeight="1">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -5937,10 +6666,14 @@
       <c r="L6" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="39" customHeight="1">
+      <c r="M6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('eastbound_south_milk_run','LAX','leg_18','1200','DFW','leg_9','800','ATL','leg_1','600','IAD'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="39" customHeight="1">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -5967,10 +6700,14 @@
       <c r="I7" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="39" customHeight="1">
+      <c r="M7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('hub_xchg_southeast','ORD','leg_25','600','ATL','leg_4','600','ORD',NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="39" customHeight="1">
       <c r="A8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -5997,10 +6734,14 @@
       <c r="I8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="39" customHeight="1">
+      <c r="M8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('hub_xchg_southwest','ORD','leg_22','800','LAX','leg_26','800','ORD',NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="39" customHeight="1">
       <c r="A9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -6027,10 +6768,14 @@
       <c r="I9" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="39" customHeight="1">
+      <c r="M9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('local_texas','IAH','leg_12','200','DAL','leg_6','200','HOU',NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="39" customHeight="1">
       <c r="A10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -6048,10 +6793,14 @@
       <c r="F10" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="39" customHeight="1">
+      <c r="M10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('northbound_east_coast','ATL','leg_3','800','JFK',NULL,NULL,NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="39" customHeight="1">
       <c r="A11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -6069,10 +6818,14 @@
       <c r="F11" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="39" customHeight="1">
+      <c r="M11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('northbound_west_coast','LAX','leg_19','1000','SEA',NULL,NULL,NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="39" customHeight="1">
       <c r="A12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -6090,10 +6843,14 @@
       <c r="F12" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="39" customHeight="1">
+      <c r="M12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('southbound_midwest','ORD','leg_21','800','DFW',NULL,NULL,NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="39" customHeight="1">
       <c r="A13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -6129,10 +6886,14 @@
       <c r="L13" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="39" customHeight="1">
+      <c r="M13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('westbound_north_milk_run','JFK','leg_16','800','ORD','leg_22','800','LAX','leg_19','1000','SEA'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="39" customHeight="1">
       <c r="A14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -6151,7 +6912,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="39" customHeight="1">
+    <row r="15" spans="1:13" ht="39" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -6171,7 +6932,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="39" customHeight="1"/>
+    <row r="16" spans="1:13" ht="39" customHeight="1"/>
     <row r="17" ht="39" customHeight="1"/>
     <row r="18" ht="39" customHeight="1"/>
     <row r="19" ht="39" customHeight="1"/>
@@ -6188,7 +6949,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{637BF729-B30E-3642-BFA4-DC44611D3A05}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39"/>
   <cols>
@@ -6235,6 +6998,15 @@
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="F2" s="1" t="str">
+        <f>"("
+&amp; IF(ISBLANK(B2),"NULL",_xlfn.CONCAT("'",B2,"'")) &amp; ","
+&amp; IF(ISBLANK(C2),"NULL",_xlfn.CONCAT("'",C2,"'")) &amp; ","
+&amp; IF(ISBLANK(D2),"NULL",_xlfn.CONCAT("'",D2,"'")) &amp; ","
+&amp; IF(ISBLANK(E2),"NULL",_xlfn.CONCAT("'",E2,"'"))
+&amp; "),"</f>
+        <v>('leg_11','600','IAD','ORD'),</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="39" customHeight="1">
       <c r="A3" s="1">
@@ -6252,6 +7024,15 @@
       <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="F3" s="1" t="str">
+        <f t="shared" ref="F3:F7" si="0">"("
+&amp; IF(ISBLANK(B3),"NULL",_xlfn.CONCAT("'",B3,"'")) &amp; ","
+&amp; IF(ISBLANK(C3),"NULL",_xlfn.CONCAT("'",C3,"'")) &amp; ","
+&amp; IF(ISBLANK(D3),"NULL",_xlfn.CONCAT("'",D3,"'")) &amp; ","
+&amp; IF(ISBLANK(E3),"NULL",_xlfn.CONCAT("'",E3,"'"))
+&amp; "),"</f>
+        <v>('leg_13','1400','IAH','LAX'),</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="39" customHeight="1">
       <c r="A4" s="1">
@@ -6269,6 +7050,10 @@
       <c r="E4" s="1" t="s">
         <v>163</v>
       </c>
+      <c r="F4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('leg_14','2400','ISP','BFI'),</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="39" customHeight="1">
       <c r="A5" s="1">
@@ -6286,6 +7071,10 @@
       <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('leg_15','800','JFK','ATL'),</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="39" customHeight="1">
       <c r="A6" s="1">
@@ -6303,6 +7092,10 @@
       <c r="E6" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="F6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('leg_2','600','ATL','IAH'),</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="39" customHeight="1">
       <c r="A7" s="1">
@@ -6319,6 +7112,10 @@
       </c>
       <c r="E7" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('leg_5','1000','BFI','LAX'),</v>
       </c>
     </row>
   </sheetData>
@@ -6332,9 +7129,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{606E67EB-3710-E942-B2B2-0BBE808B5728}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39"/>
   <cols>
@@ -6342,11 +7141,10 @@
     <col min="2" max="2" width="40.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="40.83203125" style="1" customWidth="1"/>
     <col min="4" max="8" width="29.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="39" customHeight="1">
+    <row r="1" spans="1:9" ht="39" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6372,9 +7170,8 @@
         <v>352</v>
       </c>
       <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="39" customHeight="1">
+    </row>
+    <row r="2" spans="1:9" ht="39" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -6396,12 +7193,23 @@
       <c r="G2" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>0.60416666666666663</v>
       </c>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" ht="39" customHeight="1">
+      <c r="I2" s="1" t="str">
+        <f>"("
+&amp; IF(ISBLANK(B2),"NULL",_xlfn.CONCAT("'",B2,"'")) &amp; ","
+&amp; IF(ISBLANK(C2),"NULL",_xlfn.CONCAT("'",C2,"'")) &amp; ","
+&amp; IF(ISBLANK(D2),"NULL",_xlfn.CONCAT("'",D2,"'")) &amp; ","
+&amp; IF(ISBLANK(E2),"NULL",_xlfn.CONCAT("'",E2,"'")) &amp; ","
+&amp; IF(ISBLANK(F2),"NULL",_xlfn.CONCAT("'",F2,"'")) &amp; ","
+&amp; IF(ISBLANK(G2),"NULL",_xlfn.CONCAT("'",G2,"'")) &amp; ","
+&amp; IF(ISBLANK(H2),"NULL",_xlfn.CONCAT("'",H2,"'"))
+&amp; "),"</f>
+        <v>('AM_1523','circle_west_coast','American','n330ss','2','on_ground','0.604166666666667'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="39" customHeight="1">
       <c r="A3" s="1">
         <f>A2 + 1</f>
         <v>2</v>
@@ -6424,14 +7232,25 @@
       <c r="G3" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" ht="39" customHeight="1">
+      <c r="I3" s="1" t="str">
+        <f t="shared" ref="I3:I10" si="0">"("
+&amp; IF(ISBLANK(B3),"NULL",_xlfn.CONCAT("'",B3,"'")) &amp; ","
+&amp; IF(ISBLANK(C3),"NULL",_xlfn.CONCAT("'",C3,"'")) &amp; ","
+&amp; IF(ISBLANK(D3),"NULL",_xlfn.CONCAT("'",D3,"'")) &amp; ","
+&amp; IF(ISBLANK(E3),"NULL",_xlfn.CONCAT("'",E3,"'")) &amp; ","
+&amp; IF(ISBLANK(F3),"NULL",_xlfn.CONCAT("'",F3,"'")) &amp; ","
+&amp; IF(ISBLANK(G3),"NULL",_xlfn.CONCAT("'",G3,"'")) &amp; ","
+&amp; IF(ISBLANK(H3),"NULL",_xlfn.CONCAT("'",H3,"'"))
+&amp; "),"</f>
+        <v>('DL_1174','northbound_east_coast','Delta','n106js','0','on_ground','0.333333333333333'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="39" customHeight="1">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A9" si="0">A3 + 1</f>
+        <f t="shared" ref="A4:A9" si="1">A3 + 1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -6452,14 +7271,17 @@
       <c r="G4" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>0.39583333333333331</v>
       </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" ht="39" customHeight="1">
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('DL_1243','westbound_north_nonstop','Delta','n110jn','0','on_ground','0.395833333333333'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="39" customHeight="1">
       <c r="A5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -6468,12 +7290,15 @@
       <c r="C5" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" ht="39" customHeight="1">
+      <c r="H5" s="3"/>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('DL_3410','circle_east_coast',NULL,NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="39" customHeight="1">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -6494,14 +7319,17 @@
       <c r="G6" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>0.625</v>
       </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" ht="39" customHeight="1">
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('SP_1880','circle_east_coast','Spirit','n256ap','2','in_flight','0.625'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="39" customHeight="1">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -6522,14 +7350,17 @@
       <c r="G7" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>0.58333333333333337</v>
       </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" ht="39" customHeight="1">
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('SW_1776','hub_xchg_southwest','Southwest','n401fj','2','in_flight','0.583333333333333'),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="39" customHeight="1">
       <c r="A8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -6550,14 +7381,17 @@
       <c r="G8" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>0.47916666666666669</v>
       </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" ht="39" customHeight="1">
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('SW_610','local_texas','Southwest','n118fm','2','in_flight','0.479166666666667'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="39" customHeight="1">
       <c r="A9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -6578,12 +7412,15 @@
       <c r="G9" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>0.39583333333333331</v>
       </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" ht="39" customHeight="1">
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('UN_1899','eastbound_north_milk_run','United','n517ly','0','on_ground','0.395833333333333'),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="39" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -6605,11 +7442,15 @@
       <c r="G10" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>0.45833333333333331</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="39" customHeight="1">
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('UN_523','hub_xchg_southeast','United','n620la','1','in_flight','0.458333333333333'),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="39" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -6619,13 +7460,13 @@
       <c r="C11" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" ht="39" customHeight="1"/>
-    <row r="13" spans="1:10" ht="39" customHeight="1"/>
-    <row r="14" spans="1:10" ht="39" customHeight="1"/>
-    <row r="15" spans="1:10" ht="39" customHeight="1"/>
-    <row r="16" spans="1:10" ht="39" customHeight="1"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" ht="39" customHeight="1"/>
+    <row r="13" spans="1:9" ht="39" customHeight="1"/>
+    <row r="14" spans="1:9" ht="39" customHeight="1"/>
+    <row r="15" spans="1:9" ht="39" customHeight="1"/>
+    <row r="16" spans="1:9" ht="39" customHeight="1"/>
     <row r="17" ht="39" customHeight="1"/>
     <row r="18" ht="39" customHeight="1"/>
     <row r="19" ht="39" customHeight="1"/>
@@ -6640,9 +7481,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80344FDA-9427-0B40-A0F6-D5C9CB912D8B}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39"/>
   <cols>
@@ -6652,7 +7495,7 @@
     <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39" customHeight="1">
+    <row r="1" spans="1:10" ht="39" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6681,7 +7524,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1">
+    <row r="2" spans="1:10" ht="39" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -6709,8 +7552,21 @@
       <c r="I2" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="39" customHeight="1">
+      <c r="J2" s="1" t="str">
+        <f>"("
+&amp; IF(ISBLANK(B2),"NULL",_xlfn.CONCAT("'",B2,"'")) &amp; ","
+&amp; IF(ISBLANK(C2),"NULL",_xlfn.CONCAT("'",C2,"'")) &amp; ","
+&amp; IF(ISBLANK(D2),"NULL",_xlfn.CONCAT("'",D2,"'")) &amp; ","
+&amp; IF(ISBLANK(E2),"NULL",_xlfn.CONCAT("'",E2,"'")) &amp; ","
+&amp; IF(ISBLANK(F2),"NULL",_xlfn.CONCAT("'",F2,"'")) &amp; ","
+&amp; IF(ISBLANK(G2),"NULL",_xlfn.CONCAT("'",G2,"'")) &amp; ","
+&amp; IF(ISBLANK(H2),"NULL",_xlfn.CONCAT("'",H2,"'")) &amp; ","
+&amp; IF(ISBLANK(I2),"NULL",_xlfn.CONCAT("'",I2,"'"))
+&amp; "),"</f>
+        <v>('tkt_dl_1','450','DL_1174','p24','JFK','1C','2F',''),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="39" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -6739,7 +7595,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="39" customHeight="1">
+    <row r="4" spans="1:10" ht="39" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -6768,7 +7624,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="39" customHeight="1">
+    <row r="5" spans="1:10" ht="39" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -6797,7 +7653,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="39" customHeight="1">
+    <row r="6" spans="1:10" ht="39" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -6826,7 +7682,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="39" customHeight="1">
+    <row r="7" spans="1:10" ht="39" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -6855,7 +7711,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="39" customHeight="1">
+    <row r="8" spans="1:10" ht="39" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -6884,7 +7740,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="39" customHeight="1">
+    <row r="9" spans="1:10" ht="39" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -6913,7 +7769,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="39" customHeight="1">
+    <row r="10" spans="1:10" ht="39" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -6942,7 +7798,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="39" customHeight="1">
+    <row r="11" spans="1:10" ht="39" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -6971,7 +7827,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="39" customHeight="1">
+    <row r="12" spans="1:10" ht="39" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -7000,7 +7856,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="39" customHeight="1">
+    <row r="13" spans="1:10" ht="39" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -7029,7 +7885,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="39" customHeight="1">
+    <row r="14" spans="1:10" ht="39" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -7058,7 +7914,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="39" customHeight="1">
+    <row r="15" spans="1:10" ht="39" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -7087,7 +7943,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="39" customHeight="1">
+    <row r="16" spans="1:10" ht="39" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>

</xml_diff>